<commit_message>
0 < x < 200
</commit_message>
<xml_diff>
--- a/data/basis-path.xlsx
+++ b/data/basis-path.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Project\7-Golang\software-testing-experiment\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1618D7-BDCD-49FB-A8FD-BD118777FED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F91F229-25F5-4BA0-A5BB-68C7B600DFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19680" yWindow="1065" windowWidth="9315" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Scalene</t>
   </si>
@@ -40,19 +40,21 @@
   </si>
   <si>
     <t>2,2,2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>3,4,5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>2,2,3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>1,2,3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,4,5</t>
+  </si>
+  <si>
+    <t>200,4,5</t>
   </si>
 </sst>
 </file>
@@ -95,8 +97,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -377,43 +382,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>